<commit_message>
fix add data tipe produk
</commit_message>
<xml_diff>
--- a/assets/excel/Data Transaksi.xlsx
+++ b/assets/excel/Data Transaksi.xlsx
@@ -53,7 +53,7 @@
     <t>JNE-SLD001</t>
   </si>
   <si>
-    <t>2022-04-07 13:06:00</t>
+    <t>2022-04-10 17:01:00</t>
   </si>
   <si>
     <t xml:space="preserve">Jajang </t>
@@ -62,7 +62,10 @@
     <t>Irfan</t>
   </si>
   <si>
-    <t>Selesai</t>
+    <t>2022-04-04 17:01:00</t>
+  </si>
+  <si>
+    <t>Berlangsung</t>
   </si>
   <si>
     <t>JNAP-006146</t>
@@ -74,9 +77,6 @@
     <t>dimas naufal</t>
   </si>
   <si>
-    <t>Berlangsung</t>
-  </si>
-  <si>
     <t>JP741796518</t>
   </si>
   <si>
@@ -101,7 +101,7 @@
     <t>JNE-902109</t>
   </si>
   <si>
-    <t>2022-04-07 12:49:00</t>
+    <t>2022-04-11 16:47:00</t>
   </si>
   <si>
     <t>Rhadhiya Wiraga Sudrajat</t>
@@ -560,13 +560,13 @@
         <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2">
         <v>50000</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -577,31 +577,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2">
         <v>14</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="2">
         <v>40000</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -659,7 +659,7 @@
         <v>29</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2">
         <v>7</v>
@@ -671,7 +671,7 @@
         <v>20000</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>